<commit_message>
legend position, colors, save chart function, subset simulations
</commit_message>
<xml_diff>
--- a/input_variables_list/Manage_input_variables_list_IDN_v01.xlsx
+++ b/input_variables_list/Manage_input_variables_list_IDN_v01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="108">
   <si>
     <t>variable_name</t>
   </si>
@@ -664,6 +664,15 @@
   </si>
   <si>
     <t>3 dim</t>
+  </si>
+  <si>
+    <t>simulations</t>
+  </si>
+  <si>
+    <t>BaU, CC10p, CC25p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BaU, CC10p, CC25p, CC25p_exp </t>
   </si>
 </sst>
 </file>
@@ -855,14 +864,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1202,30 +1211,30 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="24" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
     </row>
     <row r="7" spans="1:3" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
     </row>
     <row r="8" spans="1:3" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
     </row>
     <row r="9" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
@@ -1239,7 +1248,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="23" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1250,14 +1259,14 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="8" t="s">
         <v>33</v>
       </c>
@@ -1475,10 +1484,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1491,19 +1500,20 @@
     <col min="7" max="7" width="15.7265625" customWidth="1"/>
     <col min="8" max="8" width="12.7265625" customWidth="1"/>
     <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="10" max="10" width="27.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="22" t="s">
         <v>34</v>
       </c>
       <c r="E1" s="21" t="s">
@@ -1521,8 +1531,11 @@
       <c r="I1" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1544,8 +1557,11 @@
       <c r="H2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F3" t="s">
         <v>18</v>
       </c>
@@ -1555,8 +1571,11 @@
       <c r="H3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F4" t="s">
         <v>20</v>
       </c>
@@ -1567,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
         <v>22</v>
       </c>
@@ -1575,7 +1594,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F6" t="s">
         <v>24</v>
       </c>
@@ -1585,8 +1604,11 @@
       <c r="H6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1612,7 +1634,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F8" t="s">
         <v>22</v>
       </c>
@@ -1620,7 +1642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1643,7 +1665,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F10" t="s">
         <v>20</v>
       </c>
@@ -1680,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1697,9 +1719,10 @@
     <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1712,7 +1735,7 @@
       <c r="D1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>34</v>
       </c>
       <c r="F1" s="21" t="s">
@@ -1730,8 +1753,11 @@
       <c r="J1" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1760,7 +1786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F3" t="s">
         <v>99</v>
       </c>
@@ -1774,7 +1800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F4" t="s">
         <v>45</v>
       </c>
@@ -1788,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
         <v>99</v>
       </c>
@@ -1802,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F6" t="s">
         <v>100</v>
       </c>
@@ -1816,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -1836,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F8" t="s">
         <v>99</v>
       </c>
@@ -1847,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -1892,8 +1918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1907,6 +1933,7 @@
     <col min="7" max="7" width="14.54296875" customWidth="1"/>
     <col min="8" max="9" width="18.453125" customWidth="1"/>
     <col min="10" max="10" width="13.54296875" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -1922,7 +1949,7 @@
       <c r="D1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>34</v>
       </c>
       <c r="F1" s="21" t="s">
@@ -1943,7 +1970,9 @@
       <c r="K1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="21"/>
+      <c r="L1" s="21" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Use labels for both simulations and variables
</commit_message>
<xml_diff>
--- a/input_variables_list/Manage_input_variables_list_IDN_v01.xlsx
+++ b/input_variables_list/Manage_input_variables_list_IDN_v01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="111">
   <si>
     <t>variable_name</t>
   </si>
@@ -673,6 +673,15 @@
   </si>
   <si>
     <t xml:space="preserve">BaU, CC10p, CC25p, CC25p_exp </t>
+  </si>
+  <si>
+    <t>my_themeNoTtl</t>
+  </si>
+  <si>
+    <t>CC25p_exp</t>
+  </si>
+  <si>
+    <t>New Sim 25</t>
   </si>
 </sst>
 </file>
@@ -1153,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1268,78 +1277,85 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="23"/>
       <c r="B12" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="23"/>
+      <c r="B13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="6"/>
-    </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C18" s="13"/>
-    </row>
-    <row r="19" spans="1:3" ht="87" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
-      <c r="C19" s="15" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C19" s="13"/>
+    </row>
+    <row r="20" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+      <c r="A20" s="14"/>
+      <c r="C20" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C20" s="13">
-        <f>- C25</f>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C21" s="13">
+        <f>- C26</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C21" s="13"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C22" s="13"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C23" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A10:A13"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C5:C8"/>
   </mergeCells>
@@ -1486,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1555,7 +1571,7 @@
         <v>60</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
         <v>106</v>
@@ -1671,6 +1687,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9:H12">
+      <formula1>$B$10:$B$13</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
@@ -1690,9 +1711,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>readme!$B$10:$B$12</xm:f>
+            <xm:f>readme!$B$10:$B$13</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H6 H9:H12</xm:sqref>
+          <xm:sqref>H2:H6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1898,7 +1919,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>readme!$B$10:$B$12</xm:f>
+            <xm:f>readme!$B$10:$B$13</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I14</xm:sqref>
         </x14:dataValidation>
@@ -2141,7 +2162,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>readme!$B$10:$B$12</xm:f>
+            <xm:f>readme!$B$10:$B$13</xm:f>
           </x14:formula1>
           <xm:sqref>J2:J5</xm:sqref>
         </x14:dataValidation>
@@ -2201,10 +2222,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2252,13 +2273,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2266,10 +2287,10 @@
         <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2277,10 +2298,10 @@
         <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2288,9 +2309,20 @@
         <v>85</v>
       </c>
       <c r="B8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="s">
         <v>89</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
additional custom chart themes
</commit_message>
<xml_diff>
--- a/input_variables_list/Manage_input_variables_list_IDN_v01.xlsx
+++ b/input_variables_list/Manage_input_variables_list_IDN_v01.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desil\Documents\GitHub\gams_plots\input_variables_list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb388321\Documents\GitHub\gams_plots\input_variables_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73631B61-6D0F-49FF-A3C8-6C50278169CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="3" r:id="rId1"/>
@@ -23,7 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'3dim'!$F$2:$F$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="108">
   <si>
     <t>variable_name</t>
   </si>
@@ -558,15 +559,6 @@
     <t>new</t>
   </si>
   <si>
-    <t>ued</t>
-  </si>
-  <si>
-    <t>ced</t>
-  </si>
-  <si>
-    <t>ape</t>
-  </si>
-  <si>
     <t>sim</t>
   </si>
   <si>
@@ -687,7 +679,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1161,21 +1153,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="102.453125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="102.42578125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1186,7 +1178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1208,7 +1200,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -1219,7 +1211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>17</v>
       </c>
@@ -1230,22 +1222,22 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
     </row>
-    <row r="7" spans="1:3" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
     </row>
-    <row r="8" spans="1:3" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
     </row>
-    <row r="9" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -1256,7 +1248,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>29</v>
       </c>
@@ -1267,28 +1259,28 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
       <c r="B13" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>34</v>
       </c>
@@ -1299,7 +1291,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>37</v>
       </c>
@@ -1310,7 +1302,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>39</v>
       </c>
@@ -1321,35 +1313,35 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="9"/>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" s="13"/>
     </row>
-    <row r="20" spans="1:3" ht="87" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="C20" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" s="13">
         <f>- C26</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="13"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" s="13"/>
     </row>
   </sheetData>
@@ -1365,22 +1357,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" customWidth="1"/>
-    <col min="4" max="4" width="102.81640625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="102.85546875" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -1394,7 +1386,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1408,7 +1400,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1422,7 +1414,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1436,7 +1428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1450,7 +1442,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1464,12 +1456,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C7" s="19">
         <v>2015</v>
@@ -1478,18 +1470,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1499,27 +1491,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" customWidth="1"/>
-    <col min="10" max="10" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1548,10 +1540,10 @@
         <v>37</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1574,10 +1566,10 @@
         <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
         <v>18</v>
       </c>
@@ -1588,10 +1580,10 @@
         <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>20</v>
       </c>
@@ -1602,7 +1594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
         <v>22</v>
       </c>
@@ -1610,21 +1602,21 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1650,7 +1642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>22</v>
       </c>
@@ -1658,7 +1650,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1675,20 +1667,20 @@
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9:H12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9:H12" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>$B$10:$B$13</formula1>
     </dataValidation>
   </dataValidations>
@@ -1697,19 +1689,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>chart_types!$B$2:$B$5</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F6 F9:F10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>readme!$B$5:$B$8</xm:f>
           </x14:formula1>
           <xm:sqref>F11:F13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
           <x14:formula1>
             <xm:f>readme!$B$10:$B$13</xm:f>
           </x14:formula1>
@@ -1722,28 +1714,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1"/>
-    <col min="4" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.26953125" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1763,7 +1755,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>26</v>
@@ -1775,10 +1767,10 @@
         <v>37</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1807,9 +1799,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H3">
         <v>2020</v>
@@ -1821,7 +1813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
         <v>45</v>
       </c>
@@ -1835,9 +1827,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1849,21 +1841,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -1883,9 +1875,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H8">
         <v>2020</v>
@@ -1894,18 +1886,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1917,13 +1909,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>readme!$B$10:$B$13</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I14</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>chart_types!$B$6:$B$8</xm:f>
           </x14:formula1>
@@ -1936,28 +1928,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" customWidth="1"/>
-    <col min="6" max="6" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="9" width="18.453125" customWidth="1"/>
-    <col min="10" max="10" width="13.54296875" customWidth="1"/>
-    <col min="12" max="12" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1977,7 +1969,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>26</v>
@@ -1992,10 +1984,10 @@
         <v>37</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -2027,9 +2019,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H3">
         <v>2020</v>
@@ -2041,7 +2033,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -2064,9 +2056,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H5">
         <v>2020</v>
@@ -2075,12 +2067,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2095,7 +2087,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>45</v>
       </c>
@@ -2109,9 +2101,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H8">
         <v>2020</v>
@@ -2120,9 +2112,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -2134,9 +2126,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -2154,19 +2146,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>chart_types!$B$6:$B$7</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000001000000}">
           <x14:formula1>
             <xm:f>readme!$B$10:$B$13</xm:f>
           </x14:formula1>
           <xm:sqref>J2:J5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000002000000}">
           <x14:formula1>
             <xm:f>chart_types!$B$6:$B$8</xm:f>
           </x14:formula1>
@@ -2179,20 +2171,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2200,40 +2192,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>79</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>74</v>
       </c>
@@ -2244,86 +2222,86 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
         <v>85</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
         <v>86</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C9" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>